<commit_message>
Se propagan los cambios a codificación.
</commit_message>
<xml_diff>
--- a/Datos/Listados_Preprocesados/ListadoInterv_Preprocesado_PLASTICA_Codificado.xlsx
+++ b/Datos/Listados_Preprocesados/ListadoInterv_Preprocesado_PLASTICA_Codificado.xlsx
@@ -1059,7 +1059,7 @@
         <v>1</v>
       </c>
       <c r="R11">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -1283,7 +1283,7 @@
         <v>2</v>
       </c>
       <c r="R15">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:18">
@@ -2851,7 +2851,7 @@
         <v>1</v>
       </c>
       <c r="R43">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="44" spans="1:18">
@@ -4027,7 +4027,7 @@
         <v>2</v>
       </c>
       <c r="R64">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="65" spans="1:18">
@@ -4979,7 +4979,7 @@
         <v>2</v>
       </c>
       <c r="R81">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="82" spans="1:18">
@@ -5147,7 +5147,7 @@
         <v>2</v>
       </c>
       <c r="R84">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="85" spans="1:18">
@@ -6155,7 +6155,7 @@
         <v>1</v>
       </c>
       <c r="R102">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="103" spans="1:18">
@@ -6211,7 +6211,7 @@
         <v>2</v>
       </c>
       <c r="R103">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="104" spans="1:18">
@@ -6267,7 +6267,7 @@
         <v>2</v>
       </c>
       <c r="R104">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="105" spans="1:18">
@@ -6323,7 +6323,7 @@
         <v>2</v>
       </c>
       <c r="R105">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="106" spans="1:18">
@@ -7499,7 +7499,7 @@
         <v>2</v>
       </c>
       <c r="R126">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="127" spans="1:18">
@@ -8059,7 +8059,7 @@
         <v>1</v>
       </c>
       <c r="R136">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="137" spans="1:18">
@@ -9403,7 +9403,7 @@
         <v>1</v>
       </c>
       <c r="R160">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="161" spans="1:18">
@@ -10747,7 +10747,7 @@
         <v>1</v>
       </c>
       <c r="R184">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="185" spans="1:18">
@@ -10803,7 +10803,7 @@
         <v>2</v>
       </c>
       <c r="R185">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="186" spans="1:18">
@@ -10971,7 +10971,7 @@
         <v>2</v>
       </c>
       <c r="R188">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="189" spans="1:18">
@@ -11867,7 +11867,7 @@
         <v>1</v>
       </c>
       <c r="R204">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="205" spans="1:18">
@@ -11923,7 +11923,7 @@
         <v>1</v>
       </c>
       <c r="R205">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="206" spans="1:18">
@@ -11979,7 +11979,7 @@
         <v>2</v>
       </c>
       <c r="R206">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="207" spans="1:18">
@@ -12427,7 +12427,7 @@
         <v>2</v>
       </c>
       <c r="R214">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="215" spans="1:18">
@@ -12595,7 +12595,7 @@
         <v>1</v>
       </c>
       <c r="R217">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="218" spans="1:18">
@@ -12931,7 +12931,7 @@
         <v>2</v>
       </c>
       <c r="R223">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="224" spans="1:18">
@@ -16179,7 +16179,7 @@
         <v>2</v>
       </c>
       <c r="R281">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="282" spans="1:18">
@@ -16235,7 +16235,7 @@
         <v>2</v>
       </c>
       <c r="R282">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="283" spans="1:18">
@@ -16347,7 +16347,7 @@
         <v>2</v>
       </c>
       <c r="R284">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="285" spans="1:18">
@@ -16403,7 +16403,7 @@
         <v>1</v>
       </c>
       <c r="R285">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="286" spans="1:18">
@@ -17019,7 +17019,7 @@
         <v>2</v>
       </c>
       <c r="R296">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="297" spans="1:18">
@@ -17411,7 +17411,7 @@
         <v>2</v>
       </c>
       <c r="R303">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="304" spans="1:18">
@@ -17691,7 +17691,7 @@
         <v>1</v>
       </c>
       <c r="R308">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="309" spans="1:18">
@@ -20043,7 +20043,7 @@
         <v>1</v>
       </c>
       <c r="R350">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="351" spans="1:18">
@@ -24131,7 +24131,7 @@
         <v>1</v>
       </c>
       <c r="R423">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="424" spans="1:18">
@@ -24579,7 +24579,7 @@
         <v>1</v>
       </c>
       <c r="R431">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="432" spans="1:18">
@@ -24803,7 +24803,7 @@
         <v>2</v>
       </c>
       <c r="R435">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="436" spans="1:18">
@@ -25979,7 +25979,7 @@
         <v>1</v>
       </c>
       <c r="R456">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="457" spans="1:18">
@@ -26035,7 +26035,7 @@
         <v>1</v>
       </c>
       <c r="R457">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="458" spans="1:18">
@@ -26595,7 +26595,7 @@
         <v>2</v>
       </c>
       <c r="R467">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="468" spans="1:18">
@@ -27043,7 +27043,7 @@
         <v>2</v>
       </c>
       <c r="R475">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="476" spans="1:18">
@@ -28387,7 +28387,7 @@
         <v>2</v>
       </c>
       <c r="R499">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="500" spans="1:18">
@@ -29115,7 +29115,7 @@
         <v>2</v>
       </c>
       <c r="R512">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="513" spans="1:18">
@@ -29227,7 +29227,7 @@
         <v>2</v>
       </c>
       <c r="R514">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="515" spans="1:18">
@@ -29283,7 +29283,7 @@
         <v>1</v>
       </c>
       <c r="R515">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="516" spans="1:18">
@@ -29787,7 +29787,7 @@
         <v>2</v>
       </c>
       <c r="R524">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="525" spans="1:18">
@@ -29843,7 +29843,7 @@
         <v>1</v>
       </c>
       <c r="R525">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="526" spans="1:18">
@@ -30739,7 +30739,7 @@
         <v>2</v>
       </c>
       <c r="R541">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="542" spans="1:18">
@@ -32699,7 +32699,7 @@
         <v>1</v>
       </c>
       <c r="R576">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="577" spans="1:18">
@@ -33483,7 +33483,7 @@
         <v>1</v>
       </c>
       <c r="R590">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="591" spans="1:18">
@@ -36227,7 +36227,7 @@
         <v>2</v>
       </c>
       <c r="R639">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="640" spans="1:18">
@@ -36731,7 +36731,7 @@
         <v>2</v>
       </c>
       <c r="R648">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="649" spans="1:18">
@@ -37907,7 +37907,7 @@
         <v>2</v>
       </c>
       <c r="R669">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="670" spans="1:18">
@@ -38747,7 +38747,7 @@
         <v>1</v>
       </c>
       <c r="R684">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="685" spans="1:18">
@@ -40539,7 +40539,7 @@
         <v>1</v>
       </c>
       <c r="R716">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="717" spans="1:18">
@@ -42499,7 +42499,7 @@
         <v>1</v>
       </c>
       <c r="R751">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="752" spans="1:18">
@@ -42891,7 +42891,7 @@
         <v>2</v>
       </c>
       <c r="R758">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="759" spans="1:18">
@@ -43283,7 +43283,7 @@
         <v>2</v>
       </c>
       <c r="R765">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="766" spans="1:18">
@@ -44123,7 +44123,7 @@
         <v>2</v>
       </c>
       <c r="R780">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="781" spans="1:18">
@@ -44179,7 +44179,7 @@
         <v>2</v>
       </c>
       <c r="R781">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="782" spans="1:18">
@@ -44795,7 +44795,7 @@
         <v>2</v>
       </c>
       <c r="R792">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="793" spans="1:18">
@@ -44851,7 +44851,7 @@
         <v>2</v>
       </c>
       <c r="R793">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="794" spans="1:18">
@@ -46083,7 +46083,7 @@
         <v>2</v>
       </c>
       <c r="R815">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="816" spans="1:18">
@@ -46251,7 +46251,7 @@
         <v>2</v>
       </c>
       <c r="R818">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="819" spans="1:18">
@@ -46307,7 +46307,7 @@
         <v>2</v>
       </c>
       <c r="R819">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="820" spans="1:18">
@@ -47259,7 +47259,7 @@
         <v>2</v>
       </c>
       <c r="R836">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="837" spans="1:18">
@@ -48715,7 +48715,7 @@
         <v>1</v>
       </c>
       <c r="R862">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="863" spans="1:18">
@@ -48771,7 +48771,7 @@
         <v>1</v>
       </c>
       <c r="R863">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="864" spans="1:18">
@@ -51571,7 +51571,7 @@
         <v>1</v>
       </c>
       <c r="R913">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="914" spans="1:18">
@@ -52019,7 +52019,7 @@
         <v>1</v>
       </c>
       <c r="R921">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="922" spans="1:18">
@@ -52355,7 +52355,7 @@
         <v>2</v>
       </c>
       <c r="R927">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="928" spans="1:18">
@@ -52579,7 +52579,7 @@
         <v>1</v>
       </c>
       <c r="R931">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="932" spans="1:18">
@@ -52915,7 +52915,7 @@
         <v>2</v>
       </c>
       <c r="R937">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="938" spans="1:18">
@@ -54035,7 +54035,7 @@
         <v>1</v>
       </c>
       <c r="R957">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="958" spans="1:18">
@@ -54091,7 +54091,7 @@
         <v>1</v>
       </c>
       <c r="R958">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="959" spans="1:18">
@@ -54427,7 +54427,7 @@
         <v>2</v>
       </c>
       <c r="R964">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="965" spans="1:18">
@@ -55267,7 +55267,7 @@
         <v>2</v>
       </c>
       <c r="R979">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="980" spans="1:18">
@@ -55323,7 +55323,7 @@
         <v>2</v>
       </c>
       <c r="R980">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="981" spans="1:18">
@@ -55379,7 +55379,7 @@
         <v>1</v>
       </c>
       <c r="R981">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="982" spans="1:18">
@@ -55435,7 +55435,7 @@
         <v>1</v>
       </c>
       <c r="R982">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="983" spans="1:18">
@@ -57115,7 +57115,7 @@
         <v>2</v>
       </c>
       <c r="R1012">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="1013" spans="1:18">
@@ -57171,7 +57171,7 @@
         <v>1</v>
       </c>
       <c r="R1013">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="1014" spans="1:18">
@@ -57899,7 +57899,7 @@
         <v>1</v>
       </c>
       <c r="R1026">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="1027" spans="1:18">
@@ -58627,7 +58627,7 @@
         <v>1</v>
       </c>
       <c r="R1039">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="1040" spans="1:18">
@@ -59579,7 +59579,7 @@
         <v>1</v>
       </c>
       <c r="R1056">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="1057" spans="1:18">
@@ -60643,7 +60643,7 @@
         <v>1</v>
       </c>
       <c r="R1075">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="1076" spans="1:18">
@@ -66131,7 +66131,7 @@
         <v>2</v>
       </c>
       <c r="R1173">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="1174" spans="1:18">
@@ -66187,7 +66187,7 @@
         <v>2</v>
       </c>
       <c r="R1174">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="1175" spans="1:18">
@@ -66243,7 +66243,7 @@
         <v>2</v>
       </c>
       <c r="R1175">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="1176" spans="1:18">
@@ -66579,7 +66579,7 @@
         <v>1</v>
       </c>
       <c r="R1181">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="1182" spans="1:18">
@@ -68035,7 +68035,7 @@
         <v>2</v>
       </c>
       <c r="R1207">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="1208" spans="1:18">
@@ -71899,7 +71899,7 @@
         <v>2</v>
       </c>
       <c r="R1276">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="1277" spans="1:18">
@@ -72851,7 +72851,7 @@
         <v>1</v>
       </c>
       <c r="R1293">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="1294" spans="1:18">
@@ -72907,7 +72907,7 @@
         <v>1</v>
       </c>
       <c r="R1294">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="1295" spans="1:18">
@@ -74531,7 +74531,7 @@
         <v>2</v>
       </c>
       <c r="R1323">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="1324" spans="1:18">
@@ -74587,7 +74587,7 @@
         <v>2</v>
       </c>
       <c r="R1324">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="1325" spans="1:18">
@@ -74643,7 +74643,7 @@
         <v>1</v>
       </c>
       <c r="R1325">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="1326" spans="1:18">
@@ -74699,7 +74699,7 @@
         <v>2</v>
       </c>
       <c r="R1326">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="1327" spans="1:18">
@@ -74755,7 +74755,7 @@
         <v>1</v>
       </c>
       <c r="R1327">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="1328" spans="1:18">
@@ -74811,7 +74811,7 @@
         <v>1</v>
       </c>
       <c r="R1328">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="1329" spans="1:18">
@@ -75091,7 +75091,7 @@
         <v>1</v>
       </c>
       <c r="R1333">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="1334" spans="1:18">
@@ -75147,7 +75147,7 @@
         <v>1</v>
       </c>
       <c r="R1334">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="1335" spans="1:18">
@@ -81419,7 +81419,7 @@
         <v>1</v>
       </c>
       <c r="R1446">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="1447" spans="1:18">
@@ -83099,7 +83099,7 @@
         <v>2</v>
       </c>
       <c r="R1476">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="1477" spans="1:18">
@@ -83155,7 +83155,7 @@
         <v>2</v>
       </c>
       <c r="R1477">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="1478" spans="1:18">
@@ -83211,7 +83211,7 @@
         <v>1</v>
       </c>
       <c r="R1478">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="1479" spans="1:18">
@@ -84499,7 +84499,7 @@
         <v>1</v>
       </c>
       <c r="R1501">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="1502" spans="1:18">
@@ -84723,7 +84723,7 @@
         <v>1</v>
       </c>
       <c r="R1505">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="1506" spans="1:18">
@@ -86739,7 +86739,7 @@
         <v>2</v>
       </c>
       <c r="R1541">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="1542" spans="1:18">
@@ -88027,7 +88027,7 @@
         <v>1</v>
       </c>
       <c r="R1564">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="1565" spans="1:18">
@@ -89427,7 +89427,7 @@
         <v>2</v>
       </c>
       <c r="R1589">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="1590" spans="1:18">
@@ -89539,7 +89539,7 @@
         <v>1</v>
       </c>
       <c r="R1591">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="1592" spans="1:18">
@@ -90379,7 +90379,7 @@
         <v>1</v>
       </c>
       <c r="R1606">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="1607" spans="1:18">
@@ -92955,7 +92955,7 @@
         <v>1</v>
       </c>
       <c r="R1652">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="1653" spans="1:18">
@@ -93515,7 +93515,7 @@
         <v>2</v>
       </c>
       <c r="R1662">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="1663" spans="1:18">
@@ -94243,7 +94243,7 @@
         <v>1</v>
       </c>
       <c r="R1675">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="1676" spans="1:18">
@@ -96091,7 +96091,7 @@
         <v>1</v>
       </c>
       <c r="R1708">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="1709" spans="1:18">
@@ -96147,7 +96147,7 @@
         <v>2</v>
       </c>
       <c r="R1709">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="1710" spans="1:18">
@@ -98387,7 +98387,7 @@
         <v>2</v>
       </c>
       <c r="R1749">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="1750" spans="1:18">
@@ -98499,7 +98499,7 @@
         <v>2</v>
       </c>
       <c r="R1751">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="1752" spans="1:18">
@@ -98947,7 +98947,7 @@
         <v>2</v>
       </c>
       <c r="R1759">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="1760" spans="1:18">
@@ -99171,7 +99171,7 @@
         <v>1</v>
       </c>
       <c r="R1763">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="1764" spans="1:18">
@@ -99227,7 +99227,7 @@
         <v>1</v>
       </c>
       <c r="R1764">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="1765" spans="1:18">
@@ -99283,7 +99283,7 @@
         <v>1</v>
       </c>
       <c r="R1765">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="1766" spans="1:18">
@@ -99843,7 +99843,7 @@
         <v>2</v>
       </c>
       <c r="R1775">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="1776" spans="1:18">
@@ -100683,7 +100683,7 @@
         <v>2</v>
       </c>
       <c r="R1790">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="1791" spans="1:18">
@@ -102811,7 +102811,7 @@
         <v>1</v>
       </c>
       <c r="R1828">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="1829" spans="1:18">

</xml_diff>